<commit_message>
Updated salary_prediction.py by merging salaries and stats data
</commit_message>
<xml_diff>
--- a/Data/11Summary.xlsx
+++ b/Data/11Summary.xlsx
@@ -1,19 +1,488 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\Projects\Kitchener Rangers\Code Samples\Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88CF9389-B3BB-4373-B742-F833C9E6CE0E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="152">
+  <si>
+    <t>Player</t>
+  </si>
+  <si>
+    <t>Season</t>
+  </si>
+  <si>
+    <t>Team</t>
+  </si>
+  <si>
+    <t>S/C</t>
+  </si>
+  <si>
+    <t>Pos</t>
+  </si>
+  <si>
+    <t>GP</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>+/-</t>
+  </si>
+  <si>
+    <t>PIM</t>
+  </si>
+  <si>
+    <t>P/GP</t>
+  </si>
+  <si>
+    <t>EVG</t>
+  </si>
+  <si>
+    <t>EVP</t>
+  </si>
+  <si>
+    <t>PPG</t>
+  </si>
+  <si>
+    <t>PPP</t>
+  </si>
+  <si>
+    <t>SHG</t>
+  </si>
+  <si>
+    <t>SHP</t>
+  </si>
+  <si>
+    <t>OTG</t>
+  </si>
+  <si>
+    <t>GWG</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>S%</t>
+  </si>
+  <si>
+    <t>TOI/GP</t>
+  </si>
+  <si>
+    <t>FOW%</t>
+  </si>
+  <si>
+    <t>Daniel Sedin</t>
+  </si>
+  <si>
+    <t>VAN</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>18:33</t>
+  </si>
+  <si>
+    <t>Martin St. Louis</t>
+  </si>
+  <si>
+    <t>TBL</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>20:59</t>
+  </si>
+  <si>
+    <t>Corey Perry</t>
+  </si>
+  <si>
+    <t>ANA</t>
+  </si>
+  <si>
+    <t>22:19</t>
+  </si>
+  <si>
+    <t>Henrik Sedin</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>19:16</t>
+  </si>
+  <si>
+    <t>Steven Stamkos</t>
+  </si>
+  <si>
+    <t>20:12</t>
+  </si>
+  <si>
+    <t>Jarome Iginla</t>
+  </si>
+  <si>
+    <t>CGY</t>
+  </si>
+  <si>
+    <t>20:56</t>
+  </si>
+  <si>
+    <t>Alex Ovechkin</t>
+  </si>
+  <si>
+    <t>WSH</t>
+  </si>
+  <si>
+    <t>21:22</t>
+  </si>
+  <si>
+    <t>Teemu Selanne</t>
+  </si>
+  <si>
+    <t>17:56</t>
+  </si>
+  <si>
+    <t>Henrik Zetterberg</t>
+  </si>
+  <si>
+    <t>DET</t>
+  </si>
+  <si>
+    <t>19:35</t>
+  </si>
+  <si>
+    <t>Brad Richards</t>
+  </si>
+  <si>
+    <t>DAL</t>
+  </si>
+  <si>
+    <t>21:43</t>
+  </si>
+  <si>
+    <t>Eric Staal</t>
+  </si>
+  <si>
+    <t>CAR</t>
+  </si>
+  <si>
+    <t>21:56</t>
+  </si>
+  <si>
+    <t>Jonathan Toews</t>
+  </si>
+  <si>
+    <t>CHI</t>
+  </si>
+  <si>
+    <t>20:46</t>
+  </si>
+  <si>
+    <t>Claude Giroux</t>
+  </si>
+  <si>
+    <t>PHI</t>
+  </si>
+  <si>
+    <t>19:24</t>
+  </si>
+  <si>
+    <t>Ryan Getzlaf</t>
+  </si>
+  <si>
+    <t>21:51</t>
+  </si>
+  <si>
+    <t>Ryan Kesler</t>
+  </si>
+  <si>
+    <t>20:30</t>
+  </si>
+  <si>
+    <t>Patrick Marleau</t>
+  </si>
+  <si>
+    <t>SJS</t>
+  </si>
+  <si>
+    <t>20:47</t>
+  </si>
+  <si>
+    <t>Thomas Vanek</t>
+  </si>
+  <si>
+    <t>BUF</t>
+  </si>
+  <si>
+    <t>17:21</t>
+  </si>
+  <si>
+    <t>Patrick Kane</t>
+  </si>
+  <si>
+    <t>19:17</t>
+  </si>
+  <si>
+    <t>Loui Eriksson</t>
+  </si>
+  <si>
+    <t>20:34</t>
+  </si>
+  <si>
+    <t>Anze Kopitar</t>
+  </si>
+  <si>
+    <t>LAK</t>
+  </si>
+  <si>
+    <t>21:35</t>
+  </si>
+  <si>
+    <t>Patrick Sharp</t>
+  </si>
+  <si>
+    <t>19:25</t>
+  </si>
+  <si>
+    <t>Bobby Ryan</t>
+  </si>
+  <si>
+    <t>20:11</t>
+  </si>
+  <si>
+    <t>Mike Ribeiro</t>
+  </si>
+  <si>
+    <t>19:58</t>
+  </si>
+  <si>
+    <t>Joe Thornton</t>
+  </si>
+  <si>
+    <t>19:52</t>
+  </si>
+  <si>
+    <t>Alex Tanguay</t>
+  </si>
+  <si>
+    <t>19:46</t>
+  </si>
+  <si>
+    <t>Daniel Briere</t>
+  </si>
+  <si>
+    <t>18:19</t>
+  </si>
+  <si>
+    <t>Lubomir Visnovsky</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>24:18</t>
+  </si>
+  <si>
+    <t>--</t>
+  </si>
+  <si>
+    <t>John Tavares</t>
+  </si>
+  <si>
+    <t>NYI</t>
+  </si>
+  <si>
+    <t>19:15</t>
+  </si>
+  <si>
+    <t>Matt Duchene</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t>18:57</t>
+  </si>
+  <si>
+    <t>Jeff Carter</t>
+  </si>
+  <si>
+    <t>18:15</t>
+  </si>
+  <si>
+    <t>Sidney Crosby</t>
+  </si>
+  <si>
+    <t>PIT</t>
+  </si>
+  <si>
+    <t>21:55</t>
+  </si>
+  <si>
+    <t>Rick Nash</t>
+  </si>
+  <si>
+    <t>CBJ</t>
+  </si>
+  <si>
+    <t>18:56</t>
+  </si>
+  <si>
+    <t>Mike Richards</t>
+  </si>
+  <si>
+    <t>18:53</t>
+  </si>
+  <si>
+    <t>Joe Pavelski</t>
+  </si>
+  <si>
+    <t>19:39</t>
+  </si>
+  <si>
+    <t>Nicklas Backstrom</t>
+  </si>
+  <si>
+    <t>20:36</t>
+  </si>
+  <si>
+    <t>Phil Kessel</t>
+  </si>
+  <si>
+    <t>TOR</t>
+  </si>
+  <si>
+    <t>Dany Heatley</t>
+  </si>
+  <si>
+    <t>Jeff Skinner</t>
+  </si>
+  <si>
+    <t>16:44</t>
+  </si>
+  <si>
+    <t>David Backes</t>
+  </si>
+  <si>
+    <t>STL</t>
+  </si>
+  <si>
+    <t>19:42</t>
+  </si>
+  <si>
+    <t>Milan Lucic</t>
+  </si>
+  <si>
+    <t>BOS</t>
+  </si>
+  <si>
+    <t>16:35</t>
+  </si>
+  <si>
+    <t>Ryane Clowe</t>
+  </si>
+  <si>
+    <t>17:58</t>
+  </si>
+  <si>
+    <t>Martin Havlat</t>
+  </si>
+  <si>
+    <t>MIN</t>
+  </si>
+  <si>
+    <t>18:21</t>
+  </si>
+  <si>
+    <t>Clarke MacArthur</t>
+  </si>
+  <si>
+    <t>17:07</t>
+  </si>
+  <si>
+    <t>Patrik Elias</t>
+  </si>
+  <si>
+    <t>NJD</t>
+  </si>
+  <si>
+    <t>18:38</t>
+  </si>
+  <si>
+    <t>Mikko Koivu</t>
+  </si>
+  <si>
+    <t>19:29</t>
+  </si>
+  <si>
+    <t>Nicklas Lidstrom</t>
+  </si>
+  <si>
+    <t>23:28</t>
+  </si>
+  <si>
+    <t>David Krejci</t>
+  </si>
+  <si>
+    <t>18:51</t>
+  </si>
+  <si>
+    <t>Ilya Kovalchuk</t>
+  </si>
+  <si>
+    <t>22:34</t>
+  </si>
+  <si>
+    <t>Shane Doan</t>
+  </si>
+  <si>
+    <t>PHX</t>
+  </si>
+  <si>
+    <t>Andrew Ladd</t>
+  </si>
+  <si>
+    <t>ATL</t>
+  </si>
+  <si>
+    <t>20:04</t>
+  </si>
+  <si>
+    <t>Drew Doughty</t>
+  </si>
+  <si>
+    <t>25:39</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -42,7 +511,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -50,6 +520,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -374,101 +852,104 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:X51"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:X52"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="F56" sqref="F56"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Player</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Season</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Team</v>
-      </c>
-      <c r="D1" t="str">
-        <v>S/C</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Pos</v>
-      </c>
-      <c r="F1" t="str">
-        <v>GP</v>
-      </c>
-      <c r="G1" t="str">
-        <v>G</v>
-      </c>
-      <c r="H1" t="str">
-        <v>A</v>
-      </c>
-      <c r="I1" t="str">
-        <v>P</v>
-      </c>
-      <c r="J1" t="str">
-        <v>+/-</v>
-      </c>
-      <c r="K1" t="str">
-        <v>PIM</v>
-      </c>
-      <c r="L1" t="str">
-        <v>P/GP</v>
-      </c>
-      <c r="M1" t="str">
-        <v>EVG</v>
-      </c>
-      <c r="N1" t="str">
-        <v>EVP</v>
-      </c>
-      <c r="O1" t="str">
-        <v>PPG</v>
-      </c>
-      <c r="P1" t="str">
-        <v>PPP</v>
-      </c>
-      <c r="Q1" t="str">
-        <v>SHG</v>
-      </c>
-      <c r="R1" t="str">
-        <v>SHP</v>
-      </c>
-      <c r="S1" t="str">
-        <v>OTG</v>
-      </c>
-      <c r="T1" t="str">
-        <v>GWG</v>
-      </c>
-      <c r="U1" t="str">
-        <v>S</v>
-      </c>
-      <c r="V1" t="str">
-        <v>S%</v>
-      </c>
-      <c r="W1" t="str">
-        <v>TOI/GP</v>
-      </c>
-      <c r="X1" t="str">
-        <v>FOW%</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>Daniel Sedin</v>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
       </c>
       <c r="B2">
         <v>20102011</v>
       </c>
-      <c r="C2" t="str">
-        <v>VAN</v>
-      </c>
-      <c r="D2" t="str">
-        <v>L</v>
-      </c>
-      <c r="E2" t="str">
-        <v>L</v>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
       </c>
       <c r="F2">
         <v>82</v>
@@ -521,28 +1002,28 @@
       <c r="V2">
         <v>15.4</v>
       </c>
-      <c r="W2" t="str">
-        <v>18:33</v>
+      <c r="W2" t="s">
+        <v>27</v>
       </c>
       <c r="X2">
         <v>23.5</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>Martin St. Louis</v>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>28</v>
       </c>
       <c r="B3">
         <v>20102011</v>
       </c>
-      <c r="C3" t="str">
-        <v>TBL</v>
-      </c>
-      <c r="D3" t="str">
-        <v>L</v>
-      </c>
-      <c r="E3" t="str">
-        <v>R</v>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
+        <v>30</v>
       </c>
       <c r="F3">
         <v>82</v>
@@ -595,28 +1076,28 @@
       <c r="V3">
         <v>12.2</v>
       </c>
-      <c r="W3" t="str">
-        <v>20:59</v>
+      <c r="W3" t="s">
+        <v>31</v>
       </c>
       <c r="X3">
-        <v>38.2</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Corey Perry</v>
+        <v>38.200000000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>32</v>
       </c>
       <c r="B4">
         <v>20102011</v>
       </c>
-      <c r="C4" t="str">
-        <v>ANA</v>
-      </c>
-      <c r="D4" t="str">
-        <v>R</v>
-      </c>
-      <c r="E4" t="str">
-        <v>R</v>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" t="s">
+        <v>30</v>
       </c>
       <c r="F4">
         <v>82</v>
@@ -669,28 +1150,28 @@
       <c r="V4">
         <v>17.2</v>
       </c>
-      <c r="W4" t="str">
-        <v>22:19</v>
+      <c r="W4" t="s">
+        <v>34</v>
       </c>
       <c r="X4">
         <v>40.9</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>Henrik Sedin</v>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>35</v>
       </c>
       <c r="B5">
         <v>20102011</v>
       </c>
-      <c r="C5" t="str">
-        <v>VAN</v>
-      </c>
-      <c r="D5" t="str">
-        <v>L</v>
-      </c>
-      <c r="E5" t="str">
-        <v>C</v>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" t="s">
+        <v>36</v>
       </c>
       <c r="F5">
         <v>82</v>
@@ -711,7 +1192,7 @@
         <v>40</v>
       </c>
       <c r="L5">
-        <v>1.15</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="M5">
         <v>11</v>
@@ -743,28 +1224,28 @@
       <c r="V5">
         <v>12.1</v>
       </c>
-      <c r="W5" t="str">
-        <v>19:16</v>
+      <c r="W5" t="s">
+        <v>37</v>
       </c>
       <c r="X5">
         <v>52</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>Steven Stamkos</v>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>38</v>
       </c>
       <c r="B6">
         <v>20102011</v>
       </c>
-      <c r="C6" t="str">
-        <v>TBL</v>
-      </c>
-      <c r="D6" t="str">
-        <v>R</v>
-      </c>
-      <c r="E6" t="str">
-        <v>C</v>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" t="s">
+        <v>36</v>
       </c>
       <c r="F6">
         <v>82</v>
@@ -785,7 +1266,7 @@
         <v>74</v>
       </c>
       <c r="L6">
-        <v>1.11</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="M6">
         <v>28</v>
@@ -817,28 +1298,28 @@
       <c r="V6">
         <v>16.5</v>
       </c>
-      <c r="W6" t="str">
-        <v>20:12</v>
+      <c r="W6" t="s">
+        <v>39</v>
       </c>
       <c r="X6">
         <v>46.5</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>Jarome Iginla</v>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>40</v>
       </c>
       <c r="B7">
         <v>20102011</v>
       </c>
-      <c r="C7" t="str">
-        <v>CGY</v>
-      </c>
-      <c r="D7" t="str">
-        <v>R</v>
-      </c>
-      <c r="E7" t="str">
-        <v>R</v>
+      <c r="C7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" t="s">
+        <v>30</v>
       </c>
       <c r="F7">
         <v>82</v>
@@ -891,28 +1372,28 @@
       <c r="V7">
         <v>14.9</v>
       </c>
-      <c r="W7" t="str">
-        <v>20:56</v>
+      <c r="W7" t="s">
+        <v>42</v>
       </c>
       <c r="X7">
         <v>54.1</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>Alex Ovechkin</v>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>43</v>
       </c>
       <c r="B8">
         <v>20102011</v>
       </c>
-      <c r="C8" t="str">
-        <v>WSH</v>
-      </c>
-      <c r="D8" t="str">
-        <v>R</v>
-      </c>
-      <c r="E8" t="str">
-        <v>L</v>
+      <c r="C8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" t="s">
+        <v>26</v>
       </c>
       <c r="F8">
         <v>79</v>
@@ -963,30 +1444,30 @@
         <v>367</v>
       </c>
       <c r="V8">
-        <v>8.7</v>
-      </c>
-      <c r="W8" t="str">
-        <v>21:22</v>
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="W8" t="s">
+        <v>45</v>
       </c>
       <c r="X8">
-        <v>33.3</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>Teemu Selanne</v>
+        <v>33.299999999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>46</v>
       </c>
       <c r="B9">
         <v>20102011</v>
       </c>
-      <c r="C9" t="str">
-        <v>ANA</v>
-      </c>
-      <c r="D9" t="str">
-        <v>R</v>
-      </c>
-      <c r="E9" t="str">
-        <v>R</v>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" t="s">
+        <v>30</v>
       </c>
       <c r="F9">
         <v>73</v>
@@ -1007,7 +1488,7 @@
         <v>49</v>
       </c>
       <c r="L9">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="M9">
         <v>15</v>
@@ -1039,28 +1520,28 @@
       <c r="V9">
         <v>14.6</v>
       </c>
-      <c r="W9" t="str">
-        <v>17:56</v>
+      <c r="W9" t="s">
+        <v>47</v>
       </c>
       <c r="X9">
         <v>44.5</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>Henrik Zetterberg</v>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>48</v>
       </c>
       <c r="B10">
         <v>20102011</v>
       </c>
-      <c r="C10" t="str">
-        <v>DET</v>
-      </c>
-      <c r="D10" t="str">
-        <v>L</v>
-      </c>
-      <c r="E10" t="str">
-        <v>C</v>
+      <c r="C10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" t="s">
+        <v>36</v>
       </c>
       <c r="F10">
         <v>80</v>
@@ -1113,28 +1594,28 @@
       <c r="V10">
         <v>7.8</v>
       </c>
-      <c r="W10" t="str">
-        <v>19:35</v>
+      <c r="W10" t="s">
+        <v>50</v>
       </c>
       <c r="X10">
         <v>52.4</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="str">
-        <v>Brad Richards</v>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>51</v>
       </c>
       <c r="B11">
         <v>20102011</v>
       </c>
-      <c r="C11" t="str">
-        <v>DAL</v>
-      </c>
-      <c r="D11" t="str">
-        <v>L</v>
-      </c>
-      <c r="E11" t="str">
-        <v>C</v>
+      <c r="C11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" t="s">
+        <v>36</v>
       </c>
       <c r="F11">
         <v>72</v>
@@ -1187,28 +1668,28 @@
       <c r="V11">
         <v>10.3</v>
       </c>
-      <c r="W11" t="str">
-        <v>21:43</v>
+      <c r="W11" t="s">
+        <v>53</v>
       </c>
       <c r="X11">
         <v>50.6</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="str">
-        <v>Eric Staal</v>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>54</v>
       </c>
       <c r="B12">
         <v>20102011</v>
       </c>
-      <c r="C12" t="str">
-        <v>CAR</v>
-      </c>
-      <c r="D12" t="str">
-        <v>L</v>
-      </c>
-      <c r="E12" t="str">
-        <v>C</v>
+      <c r="C12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" t="s">
+        <v>36</v>
       </c>
       <c r="F12">
         <v>81</v>
@@ -1261,28 +1742,28 @@
       <c r="V12">
         <v>11.2</v>
       </c>
-      <c r="W12" t="str">
-        <v>21:56</v>
+      <c r="W12" t="s">
+        <v>56</v>
       </c>
       <c r="X12">
         <v>48</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="str">
-        <v>Jonathan Toews</v>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>57</v>
       </c>
       <c r="B13">
         <v>20102011</v>
       </c>
-      <c r="C13" t="str">
-        <v>CHI</v>
-      </c>
-      <c r="D13" t="str">
-        <v>L</v>
-      </c>
-      <c r="E13" t="str">
-        <v>C</v>
+      <c r="C13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" t="s">
+        <v>36</v>
       </c>
       <c r="F13">
         <v>80</v>
@@ -1335,28 +1816,28 @@
       <c r="V13">
         <v>13.7</v>
       </c>
-      <c r="W13" t="str">
-        <v>20:46</v>
+      <c r="W13" t="s">
+        <v>59</v>
       </c>
       <c r="X13">
         <v>56.7</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="str">
-        <v>Claude Giroux</v>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>60</v>
       </c>
       <c r="B14">
         <v>20102011</v>
       </c>
-      <c r="C14" t="str">
-        <v>PHI</v>
-      </c>
-      <c r="D14" t="str">
-        <v>R</v>
-      </c>
-      <c r="E14" t="str">
-        <v>C</v>
+      <c r="C14" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" t="s">
+        <v>36</v>
       </c>
       <c r="F14">
         <v>82</v>
@@ -1409,28 +1890,28 @@
       <c r="V14">
         <v>14.8</v>
       </c>
-      <c r="W14" t="str">
-        <v>19:24</v>
+      <c r="W14" t="s">
+        <v>62</v>
       </c>
       <c r="X14">
         <v>50</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="str">
-        <v>Ryan Getzlaf</v>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>63</v>
       </c>
       <c r="B15">
         <v>20102011</v>
       </c>
-      <c r="C15" t="str">
-        <v>ANA</v>
-      </c>
-      <c r="D15" t="str">
-        <v>R</v>
-      </c>
-      <c r="E15" t="str">
-        <v>C</v>
+      <c r="C15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" t="s">
+        <v>36</v>
       </c>
       <c r="F15">
         <v>67</v>
@@ -1451,7 +1932,7 @@
         <v>35</v>
       </c>
       <c r="L15">
-        <v>1.13</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="M15">
         <v>12</v>
@@ -1483,28 +1964,28 @@
       <c r="V15">
         <v>16.2</v>
       </c>
-      <c r="W15" t="str">
-        <v>21:51</v>
+      <c r="W15" t="s">
+        <v>64</v>
       </c>
       <c r="X15">
         <v>45.8</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" t="str">
-        <v>Ryan Kesler</v>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>65</v>
       </c>
       <c r="B16">
         <v>20102011</v>
       </c>
-      <c r="C16" t="str">
-        <v>VAN</v>
-      </c>
-      <c r="D16" t="str">
-        <v>R</v>
-      </c>
-      <c r="E16" t="str">
-        <v>C</v>
+      <c r="C16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" t="s">
+        <v>36</v>
       </c>
       <c r="F16">
         <v>82</v>
@@ -1557,28 +2038,28 @@
       <c r="V16">
         <v>15.8</v>
       </c>
-      <c r="W16" t="str">
-        <v>20:30</v>
+      <c r="W16" t="s">
+        <v>66</v>
       </c>
       <c r="X16">
         <v>57.4</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" t="str">
-        <v>Patrick Marleau</v>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>67</v>
       </c>
       <c r="B17">
         <v>20102011</v>
       </c>
-      <c r="C17" t="str">
-        <v>SJS</v>
-      </c>
-      <c r="D17" t="str">
-        <v>L</v>
-      </c>
-      <c r="E17" t="str">
-        <v>C</v>
+      <c r="C17" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" t="s">
+        <v>36</v>
       </c>
       <c r="F17">
         <v>82</v>
@@ -1631,28 +2112,28 @@
       <c r="V17">
         <v>13.3</v>
       </c>
-      <c r="W17" t="str">
-        <v>20:47</v>
+      <c r="W17" t="s">
+        <v>69</v>
       </c>
       <c r="X17">
         <v>52.5</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" t="str">
-        <v>Thomas Vanek</v>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>70</v>
       </c>
       <c r="B18">
         <v>20102011</v>
       </c>
-      <c r="C18" t="str">
-        <v>BUF</v>
-      </c>
-      <c r="D18" t="str">
-        <v>R</v>
-      </c>
-      <c r="E18" t="str">
-        <v>L</v>
+      <c r="C18" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" t="s">
+        <v>26</v>
       </c>
       <c r="F18">
         <v>80</v>
@@ -1705,28 +2186,28 @@
       <c r="V18">
         <v>13.5</v>
       </c>
-      <c r="W18" t="str">
-        <v>17:21</v>
+      <c r="W18" t="s">
+        <v>72</v>
       </c>
       <c r="X18">
         <v>30.8</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" t="str">
-        <v>Patrick Kane</v>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>73</v>
       </c>
       <c r="B19">
         <v>20102011</v>
       </c>
-      <c r="C19" t="str">
-        <v>CHI</v>
-      </c>
-      <c r="D19" t="str">
-        <v>L</v>
-      </c>
-      <c r="E19" t="str">
-        <v>R</v>
+      <c r="C19" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" t="s">
+        <v>30</v>
       </c>
       <c r="F19">
         <v>73</v>
@@ -1779,28 +2260,28 @@
       <c r="V19">
         <v>12.5</v>
       </c>
-      <c r="W19" t="str">
-        <v>19:17</v>
+      <c r="W19" t="s">
+        <v>74</v>
       </c>
       <c r="X19">
         <v>14.3</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" t="str">
-        <v>Loui Eriksson</v>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>75</v>
       </c>
       <c r="B20">
         <v>20102011</v>
       </c>
-      <c r="C20" t="str">
-        <v>DAL</v>
-      </c>
-      <c r="D20" t="str">
-        <v>L</v>
-      </c>
-      <c r="E20" t="str">
-        <v>L</v>
+      <c r="C20" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" t="s">
+        <v>26</v>
       </c>
       <c r="F20">
         <v>79</v>
@@ -1853,28 +2334,28 @@
       <c r="V20">
         <v>15.1</v>
       </c>
-      <c r="W20" t="str">
-        <v>20:34</v>
+      <c r="W20" t="s">
+        <v>76</v>
       </c>
       <c r="X20">
         <v>25</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" t="str">
-        <v>Anze Kopitar</v>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>77</v>
       </c>
       <c r="B21">
         <v>20102011</v>
       </c>
-      <c r="C21" t="str">
-        <v>LAK</v>
-      </c>
-      <c r="D21" t="str">
-        <v>L</v>
-      </c>
-      <c r="E21" t="str">
-        <v>C</v>
+      <c r="C21" t="s">
+        <v>78</v>
+      </c>
+      <c r="D21" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" t="s">
+        <v>36</v>
       </c>
       <c r="F21">
         <v>75</v>
@@ -1927,28 +2408,28 @@
       <c r="V21">
         <v>10.7</v>
       </c>
-      <c r="W21" t="str">
-        <v>21:35</v>
+      <c r="W21" t="s">
+        <v>79</v>
       </c>
       <c r="X21">
         <v>49.9</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" t="str">
-        <v>Patrick Sharp</v>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>80</v>
       </c>
       <c r="B22">
         <v>20102011</v>
       </c>
-      <c r="C22" t="str">
-        <v>CHI</v>
-      </c>
-      <c r="D22" t="str">
-        <v>R</v>
-      </c>
-      <c r="E22" t="str">
-        <v>L</v>
+      <c r="C22" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" t="s">
+        <v>30</v>
+      </c>
+      <c r="E22" t="s">
+        <v>26</v>
       </c>
       <c r="F22">
         <v>74</v>
@@ -2001,28 +2482,28 @@
       <c r="V22">
         <v>12.7</v>
       </c>
-      <c r="W22" t="str">
-        <v>19:25</v>
+      <c r="W22" t="s">
+        <v>81</v>
       </c>
       <c r="X22">
         <v>48</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" t="str">
-        <v>Bobby Ryan</v>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>82</v>
       </c>
       <c r="B23">
         <v>20102011</v>
       </c>
-      <c r="C23" t="str">
-        <v>ANA</v>
-      </c>
-      <c r="D23" t="str">
-        <v>R</v>
-      </c>
-      <c r="E23" t="str">
-        <v>R</v>
+      <c r="C23" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" t="s">
+        <v>30</v>
+      </c>
+      <c r="E23" t="s">
+        <v>30</v>
       </c>
       <c r="F23">
         <v>82</v>
@@ -2075,28 +2556,28 @@
       <c r="V23">
         <v>12.6</v>
       </c>
-      <c r="W23" t="str">
-        <v>20:11</v>
+      <c r="W23" t="s">
+        <v>83</v>
       </c>
       <c r="X23">
-        <v>39.7</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="str">
-        <v>Mike Ribeiro</v>
+        <v>39.700000000000003</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>84</v>
       </c>
       <c r="B24">
         <v>20102011</v>
       </c>
-      <c r="C24" t="str">
-        <v>DAL</v>
-      </c>
-      <c r="D24" t="str">
-        <v>L</v>
-      </c>
-      <c r="E24" t="str">
-        <v>C</v>
+      <c r="C24" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24" t="s">
+        <v>26</v>
+      </c>
+      <c r="E24" t="s">
+        <v>36</v>
       </c>
       <c r="F24">
         <v>82</v>
@@ -2149,28 +2630,28 @@
       <c r="V24">
         <v>11.8</v>
       </c>
-      <c r="W24" t="str">
-        <v>19:58</v>
+      <c r="W24" t="s">
+        <v>85</v>
       </c>
       <c r="X24">
         <v>46.6</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" t="str">
-        <v>Joe Thornton</v>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>86</v>
       </c>
       <c r="B25">
         <v>20102011</v>
       </c>
-      <c r="C25" t="str">
-        <v>SJS</v>
-      </c>
-      <c r="D25" t="str">
-        <v>L</v>
-      </c>
-      <c r="E25" t="str">
-        <v>C</v>
+      <c r="C25" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" t="s">
+        <v>36</v>
       </c>
       <c r="F25">
         <v>80</v>
@@ -2223,28 +2704,28 @@
       <c r="V25">
         <v>14.1</v>
       </c>
-      <c r="W25" t="str">
-        <v>19:52</v>
+      <c r="W25" t="s">
+        <v>87</v>
       </c>
       <c r="X25">
         <v>54.4</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" t="str">
-        <v>Alex Tanguay</v>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>88</v>
       </c>
       <c r="B26">
         <v>20102011</v>
       </c>
-      <c r="C26" t="str">
-        <v>CGY</v>
-      </c>
-      <c r="D26" t="str">
-        <v>L</v>
-      </c>
-      <c r="E26" t="str">
-        <v>L</v>
+      <c r="C26" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" t="s">
+        <v>26</v>
+      </c>
+      <c r="E26" t="s">
+        <v>26</v>
       </c>
       <c r="F26">
         <v>79</v>
@@ -2297,28 +2778,28 @@
       <c r="V26">
         <v>18.3</v>
       </c>
-      <c r="W26" t="str">
-        <v>19:46</v>
+      <c r="W26" t="s">
+        <v>89</v>
       </c>
       <c r="X26">
-        <v>39.3</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="str">
-        <v>Daniel Briere</v>
+        <v>39.299999999999997</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>90</v>
       </c>
       <c r="B27">
         <v>20102011</v>
       </c>
-      <c r="C27" t="str">
-        <v>PHI</v>
-      </c>
-      <c r="D27" t="str">
-        <v>R</v>
-      </c>
-      <c r="E27" t="str">
-        <v>C</v>
+      <c r="C27" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27" t="s">
+        <v>30</v>
+      </c>
+      <c r="E27" t="s">
+        <v>36</v>
       </c>
       <c r="F27">
         <v>77</v>
@@ -2371,28 +2852,28 @@
       <c r="V27">
         <v>13.8</v>
       </c>
-      <c r="W27" t="str">
-        <v>18:19</v>
+      <c r="W27" t="s">
+        <v>91</v>
       </c>
       <c r="X27">
         <v>48.2</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" t="str">
-        <v>Lubomir Visnovsky</v>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>92</v>
       </c>
       <c r="B28">
         <v>20102011</v>
       </c>
-      <c r="C28" t="str">
-        <v>ANA</v>
-      </c>
-      <c r="D28" t="str">
-        <v>L</v>
-      </c>
-      <c r="E28" t="str">
-        <v>D</v>
+      <c r="C28" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" t="s">
+        <v>26</v>
+      </c>
+      <c r="E28" t="s">
+        <v>93</v>
       </c>
       <c r="F28">
         <v>81</v>
@@ -2445,28 +2926,28 @@
       <c r="V28">
         <v>11.8</v>
       </c>
-      <c r="W28" t="str">
-        <v>24:18</v>
-      </c>
-      <c r="X28" t="str">
-        <v>--</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="str">
-        <v>John Tavares</v>
+      <c r="W28" t="s">
+        <v>94</v>
+      </c>
+      <c r="X28" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>96</v>
       </c>
       <c r="B29">
         <v>20102011</v>
       </c>
-      <c r="C29" t="str">
-        <v>NYI</v>
-      </c>
-      <c r="D29" t="str">
-        <v>L</v>
-      </c>
-      <c r="E29" t="str">
-        <v>C</v>
+      <c r="C29" t="s">
+        <v>97</v>
+      </c>
+      <c r="D29" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" t="s">
+        <v>36</v>
       </c>
       <c r="F29">
         <v>79</v>
@@ -2519,28 +3000,28 @@
       <c r="V29">
         <v>11.9</v>
       </c>
-      <c r="W29" t="str">
-        <v>19:15</v>
+      <c r="W29" t="s">
+        <v>98</v>
       </c>
       <c r="X29">
         <v>52.5</v>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" t="str">
-        <v>Matt Duchene</v>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>99</v>
       </c>
       <c r="B30">
         <v>20102011</v>
       </c>
-      <c r="C30" t="str">
-        <v>COL</v>
-      </c>
-      <c r="D30" t="str">
-        <v>L</v>
-      </c>
-      <c r="E30" t="str">
-        <v>C</v>
+      <c r="C30" t="s">
+        <v>100</v>
+      </c>
+      <c r="D30" t="s">
+        <v>26</v>
+      </c>
+      <c r="E30" t="s">
+        <v>36</v>
       </c>
       <c r="F30">
         <v>80</v>
@@ -2593,28 +3074,28 @@
       <c r="V30">
         <v>13.4</v>
       </c>
-      <c r="W30" t="str">
-        <v>18:57</v>
+      <c r="W30" t="s">
+        <v>101</v>
       </c>
       <c r="X30">
         <v>50.4</v>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" t="str">
-        <v>Jeff Carter</v>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>102</v>
       </c>
       <c r="B31">
         <v>20102011</v>
       </c>
-      <c r="C31" t="str">
-        <v>PHI</v>
-      </c>
-      <c r="D31" t="str">
-        <v>R</v>
-      </c>
-      <c r="E31" t="str">
-        <v>C</v>
+      <c r="C31" t="s">
+        <v>61</v>
+      </c>
+      <c r="D31" t="s">
+        <v>30</v>
+      </c>
+      <c r="E31" t="s">
+        <v>36</v>
       </c>
       <c r="F31">
         <v>80</v>
@@ -2667,28 +3148,28 @@
       <c r="V31">
         <v>10.8</v>
       </c>
-      <c r="W31" t="str">
-        <v>18:15</v>
+      <c r="W31" t="s">
+        <v>103</v>
       </c>
       <c r="X31">
         <v>54.7</v>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" t="str">
-        <v>Sidney Crosby</v>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>104</v>
       </c>
       <c r="B32">
         <v>20102011</v>
       </c>
-      <c r="C32" t="str">
-        <v>PIT</v>
-      </c>
-      <c r="D32" t="str">
-        <v>L</v>
-      </c>
-      <c r="E32" t="str">
-        <v>C</v>
+      <c r="C32" t="s">
+        <v>105</v>
+      </c>
+      <c r="D32" t="s">
+        <v>26</v>
+      </c>
+      <c r="E32" t="s">
+        <v>36</v>
       </c>
       <c r="F32">
         <v>41</v>
@@ -2739,30 +3220,30 @@
         <v>161</v>
       </c>
       <c r="V32">
-        <v>19.9</v>
-      </c>
-      <c r="W32" t="str">
-        <v>21:55</v>
+        <v>19.899999999999999</v>
+      </c>
+      <c r="W32" t="s">
+        <v>106</v>
       </c>
       <c r="X32">
         <v>55.7</v>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" t="str">
-        <v>Rick Nash</v>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>107</v>
       </c>
       <c r="B33">
         <v>20102011</v>
       </c>
-      <c r="C33" t="str">
-        <v>CBJ</v>
-      </c>
-      <c r="D33" t="str">
-        <v>L</v>
-      </c>
-      <c r="E33" t="str">
-        <v>L</v>
+      <c r="C33" t="s">
+        <v>108</v>
+      </c>
+      <c r="D33" t="s">
+        <v>26</v>
+      </c>
+      <c r="E33" t="s">
+        <v>26</v>
       </c>
       <c r="F33">
         <v>75</v>
@@ -2815,28 +3296,28 @@
       <c r="V33">
         <v>10.5</v>
       </c>
-      <c r="W33" t="str">
-        <v>18:56</v>
+      <c r="W33" t="s">
+        <v>109</v>
       </c>
       <c r="X33">
         <v>29.2</v>
       </c>
     </row>
-    <row r="34">
-      <c r="A34" t="str">
-        <v>Mike Richards</v>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>110</v>
       </c>
       <c r="B34">
         <v>20102011</v>
       </c>
-      <c r="C34" t="str">
-        <v>PHI</v>
-      </c>
-      <c r="D34" t="str">
-        <v>L</v>
-      </c>
-      <c r="E34" t="str">
-        <v>C</v>
+      <c r="C34" t="s">
+        <v>61</v>
+      </c>
+      <c r="D34" t="s">
+        <v>26</v>
+      </c>
+      <c r="E34" t="s">
+        <v>36</v>
       </c>
       <c r="F34">
         <v>81</v>
@@ -2889,28 +3370,28 @@
       <c r="V34">
         <v>12.5</v>
       </c>
-      <c r="W34" t="str">
-        <v>18:53</v>
+      <c r="W34" t="s">
+        <v>111</v>
       </c>
       <c r="X34">
         <v>49.8</v>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" t="str">
-        <v>Joe Pavelski</v>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>112</v>
       </c>
       <c r="B35">
         <v>20102011</v>
       </c>
-      <c r="C35" t="str">
-        <v>SJS</v>
-      </c>
-      <c r="D35" t="str">
-        <v>R</v>
-      </c>
-      <c r="E35" t="str">
-        <v>C</v>
+      <c r="C35" t="s">
+        <v>68</v>
+      </c>
+      <c r="D35" t="s">
+        <v>30</v>
+      </c>
+      <c r="E35" t="s">
+        <v>36</v>
       </c>
       <c r="F35">
         <v>74</v>
@@ -2963,28 +3444,28 @@
       <c r="V35">
         <v>7.1</v>
       </c>
-      <c r="W35" t="str">
-        <v>19:39</v>
+      <c r="W35" t="s">
+        <v>113</v>
       </c>
       <c r="X35">
         <v>54.3</v>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" t="str">
-        <v>Nicklas Backstrom</v>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>114</v>
       </c>
       <c r="B36">
         <v>20102011</v>
       </c>
-      <c r="C36" t="str">
-        <v>WSH</v>
-      </c>
-      <c r="D36" t="str">
-        <v>L</v>
-      </c>
-      <c r="E36" t="str">
-        <v>C</v>
+      <c r="C36" t="s">
+        <v>44</v>
+      </c>
+      <c r="D36" t="s">
+        <v>26</v>
+      </c>
+      <c r="E36" t="s">
+        <v>36</v>
       </c>
       <c r="F36">
         <v>77</v>
@@ -3037,28 +3518,28 @@
       <c r="V36">
         <v>8.9</v>
       </c>
-      <c r="W36" t="str">
-        <v>20:36</v>
+      <c r="W36" t="s">
+        <v>115</v>
       </c>
       <c r="X36">
         <v>52.5</v>
       </c>
     </row>
-    <row r="37">
-      <c r="A37" t="str">
-        <v>Phil Kessel</v>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>116</v>
       </c>
       <c r="B37">
         <v>20102011</v>
       </c>
-      <c r="C37" t="str">
-        <v>TOR</v>
-      </c>
-      <c r="D37" t="str">
-        <v>R</v>
-      </c>
-      <c r="E37" t="str">
-        <v>R</v>
+      <c r="C37" t="s">
+        <v>117</v>
+      </c>
+      <c r="D37" t="s">
+        <v>30</v>
+      </c>
+      <c r="E37" t="s">
+        <v>30</v>
       </c>
       <c r="F37">
         <v>82</v>
@@ -3111,28 +3592,28 @@
       <c r="V37">
         <v>9.9</v>
       </c>
-      <c r="W37" t="str">
-        <v>19:39</v>
+      <c r="W37" t="s">
+        <v>113</v>
       </c>
       <c r="X37">
-        <v>40.7</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="str">
-        <v>Dany Heatley</v>
+        <v>40.700000000000003</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>118</v>
       </c>
       <c r="B38">
         <v>20102011</v>
       </c>
-      <c r="C38" t="str">
-        <v>SJS</v>
-      </c>
-      <c r="D38" t="str">
-        <v>L</v>
-      </c>
-      <c r="E38" t="str">
-        <v>L</v>
+      <c r="C38" t="s">
+        <v>68</v>
+      </c>
+      <c r="D38" t="s">
+        <v>26</v>
+      </c>
+      <c r="E38" t="s">
+        <v>26</v>
       </c>
       <c r="F38">
         <v>80</v>
@@ -3185,28 +3666,28 @@
       <c r="V38">
         <v>12</v>
       </c>
-      <c r="W38" t="str">
-        <v>19:39</v>
+      <c r="W38" t="s">
+        <v>113</v>
       </c>
       <c r="X38">
         <v>45</v>
       </c>
     </row>
-    <row r="39">
-      <c r="A39" t="str">
-        <v>Jeff Skinner</v>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>119</v>
       </c>
       <c r="B39">
         <v>20102011</v>
       </c>
-      <c r="C39" t="str">
-        <v>CAR</v>
-      </c>
-      <c r="D39" t="str">
-        <v>L</v>
-      </c>
-      <c r="E39" t="str">
-        <v>L</v>
+      <c r="C39" t="s">
+        <v>55</v>
+      </c>
+      <c r="D39" t="s">
+        <v>26</v>
+      </c>
+      <c r="E39" t="s">
+        <v>26</v>
       </c>
       <c r="F39">
         <v>82</v>
@@ -3259,28 +3740,28 @@
       <c r="V39">
         <v>14.4</v>
       </c>
-      <c r="W39" t="str">
-        <v>16:44</v>
+      <c r="W39" t="s">
+        <v>120</v>
       </c>
       <c r="X39">
         <v>36.9</v>
       </c>
     </row>
-    <row r="40">
-      <c r="A40" t="str">
-        <v>David Backes</v>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>121</v>
       </c>
       <c r="B40">
         <v>20102011</v>
       </c>
-      <c r="C40" t="str">
-        <v>STL</v>
-      </c>
-      <c r="D40" t="str">
-        <v>R</v>
-      </c>
-      <c r="E40" t="str">
-        <v>R</v>
+      <c r="C40" t="s">
+        <v>122</v>
+      </c>
+      <c r="D40" t="s">
+        <v>30</v>
+      </c>
+      <c r="E40" t="s">
+        <v>30</v>
       </c>
       <c r="F40">
         <v>82</v>
@@ -3333,28 +3814,28 @@
       <c r="V40">
         <v>14.7</v>
       </c>
-      <c r="W40" t="str">
-        <v>19:42</v>
+      <c r="W40" t="s">
+        <v>123</v>
       </c>
       <c r="X40">
         <v>44.5</v>
       </c>
     </row>
-    <row r="41">
-      <c r="A41" t="str">
-        <v>Milan Lucic</v>
+    <row r="41" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>124</v>
       </c>
       <c r="B41">
         <v>20102011</v>
       </c>
-      <c r="C41" t="str">
-        <v>BOS</v>
-      </c>
-      <c r="D41" t="str">
-        <v>L</v>
-      </c>
-      <c r="E41" t="str">
-        <v>L</v>
+      <c r="C41" t="s">
+        <v>125</v>
+      </c>
+      <c r="D41" t="s">
+        <v>26</v>
+      </c>
+      <c r="E41" t="s">
+        <v>26</v>
       </c>
       <c r="F41">
         <v>79</v>
@@ -3407,28 +3888,28 @@
       <c r="V41">
         <v>17.3</v>
       </c>
-      <c r="W41" t="str">
-        <v>16:35</v>
+      <c r="W41" t="s">
+        <v>126</v>
       </c>
       <c r="X41">
         <v>38.9</v>
       </c>
     </row>
-    <row r="42">
-      <c r="A42" t="str">
-        <v>Ryane Clowe</v>
+    <row r="42" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>127</v>
       </c>
       <c r="B42">
         <v>20102011</v>
       </c>
-      <c r="C42" t="str">
-        <v>SJS</v>
-      </c>
-      <c r="D42" t="str">
-        <v>L</v>
-      </c>
-      <c r="E42" t="str">
-        <v>L</v>
+      <c r="C42" t="s">
+        <v>68</v>
+      </c>
+      <c r="D42" t="s">
+        <v>26</v>
+      </c>
+      <c r="E42" t="s">
+        <v>26</v>
       </c>
       <c r="F42">
         <v>75</v>
@@ -3481,28 +3962,28 @@
       <c r="V42">
         <v>13</v>
       </c>
-      <c r="W42" t="str">
-        <v>17:58</v>
+      <c r="W42" t="s">
+        <v>128</v>
       </c>
       <c r="X42">
         <v>41.5</v>
       </c>
     </row>
-    <row r="43">
-      <c r="A43" t="str">
-        <v>Martin Havlat</v>
+    <row r="43" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>129</v>
       </c>
       <c r="B43">
         <v>20102011</v>
       </c>
-      <c r="C43" t="str">
-        <v>MIN</v>
-      </c>
-      <c r="D43" t="str">
-        <v>L</v>
-      </c>
-      <c r="E43" t="str">
-        <v>R</v>
+      <c r="C43" t="s">
+        <v>130</v>
+      </c>
+      <c r="D43" t="s">
+        <v>26</v>
+      </c>
+      <c r="E43" t="s">
+        <v>30</v>
       </c>
       <c r="F43">
         <v>78</v>
@@ -3555,28 +4036,28 @@
       <c r="V43">
         <v>9.6</v>
       </c>
-      <c r="W43" t="str">
-        <v>18:21</v>
+      <c r="W43" t="s">
+        <v>131</v>
       </c>
       <c r="X43">
         <v>30</v>
       </c>
     </row>
-    <row r="44">
-      <c r="A44" t="str">
-        <v>Clarke MacArthur</v>
+    <row r="44" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>132</v>
       </c>
       <c r="B44">
         <v>20102011</v>
       </c>
-      <c r="C44" t="str">
-        <v>TOR</v>
-      </c>
-      <c r="D44" t="str">
-        <v>L</v>
-      </c>
-      <c r="E44" t="str">
-        <v>L</v>
+      <c r="C44" t="s">
+        <v>117</v>
+      </c>
+      <c r="D44" t="s">
+        <v>26</v>
+      </c>
+      <c r="E44" t="s">
+        <v>26</v>
       </c>
       <c r="F44">
         <v>82</v>
@@ -3629,28 +4110,28 @@
       <c r="V44">
         <v>13.6</v>
       </c>
-      <c r="W44" t="str">
-        <v>17:07</v>
+      <c r="W44" t="s">
+        <v>133</v>
       </c>
       <c r="X44">
         <v>56.3</v>
       </c>
     </row>
-    <row r="45">
-      <c r="A45" t="str">
-        <v>Patrik Elias</v>
+    <row r="45" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>134</v>
       </c>
       <c r="B45">
         <v>20102011</v>
       </c>
-      <c r="C45" t="str">
-        <v>NJD</v>
-      </c>
-      <c r="D45" t="str">
-        <v>L</v>
-      </c>
-      <c r="E45" t="str">
-        <v>C</v>
+      <c r="C45" t="s">
+        <v>135</v>
+      </c>
+      <c r="D45" t="s">
+        <v>26</v>
+      </c>
+      <c r="E45" t="s">
+        <v>36</v>
       </c>
       <c r="F45">
         <v>81</v>
@@ -3703,28 +4184,28 @@
       <c r="V45">
         <v>10.3</v>
       </c>
-      <c r="W45" t="str">
-        <v>18:38</v>
+      <c r="W45" t="s">
+        <v>136</v>
       </c>
       <c r="X45">
         <v>45</v>
       </c>
     </row>
-    <row r="46">
-      <c r="A46" t="str">
-        <v>Mikko Koivu</v>
+    <row r="46" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>137</v>
       </c>
       <c r="B46">
         <v>20102011</v>
       </c>
-      <c r="C46" t="str">
-        <v>MIN</v>
-      </c>
-      <c r="D46" t="str">
-        <v>L</v>
-      </c>
-      <c r="E46" t="str">
-        <v>C</v>
+      <c r="C46" t="s">
+        <v>130</v>
+      </c>
+      <c r="D46" t="s">
+        <v>26</v>
+      </c>
+      <c r="E46" t="s">
+        <v>36</v>
       </c>
       <c r="F46">
         <v>71</v>
@@ -3777,28 +4258,28 @@
       <c r="V46">
         <v>8.9</v>
       </c>
-      <c r="W46" t="str">
-        <v>19:29</v>
+      <c r="W46" t="s">
+        <v>138</v>
       </c>
       <c r="X46">
         <v>52.8</v>
       </c>
     </row>
-    <row r="47">
-      <c r="A47" t="str">
-        <v>Nicklas Lidstrom</v>
+    <row r="47" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>139</v>
       </c>
       <c r="B47">
         <v>20102011</v>
       </c>
-      <c r="C47" t="str">
-        <v>DET</v>
-      </c>
-      <c r="D47" t="str">
-        <v>L</v>
-      </c>
-      <c r="E47" t="str">
-        <v>D</v>
+      <c r="C47" t="s">
+        <v>49</v>
+      </c>
+      <c r="D47" t="s">
+        <v>26</v>
+      </c>
+      <c r="E47" t="s">
+        <v>93</v>
       </c>
       <c r="F47">
         <v>82</v>
@@ -3851,28 +4332,28 @@
       <c r="V47">
         <v>9.1</v>
       </c>
-      <c r="W47" t="str">
-        <v>23:28</v>
-      </c>
-      <c r="X47" t="str">
-        <v>--</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="str">
-        <v>David Krejci</v>
+      <c r="W47" t="s">
+        <v>140</v>
+      </c>
+      <c r="X47" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="48" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>141</v>
       </c>
       <c r="B48">
         <v>20102011</v>
       </c>
-      <c r="C48" t="str">
-        <v>BOS</v>
-      </c>
-      <c r="D48" t="str">
-        <v>R</v>
-      </c>
-      <c r="E48" t="str">
-        <v>C</v>
+      <c r="C48" t="s">
+        <v>125</v>
+      </c>
+      <c r="D48" t="s">
+        <v>30</v>
+      </c>
+      <c r="E48" t="s">
+        <v>36</v>
       </c>
       <c r="F48">
         <v>75</v>
@@ -3923,30 +4404,30 @@
         <v>157</v>
       </c>
       <c r="V48">
-        <v>8.3</v>
-      </c>
-      <c r="W48" t="str">
-        <v>18:51</v>
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="W48" t="s">
+        <v>142</v>
       </c>
       <c r="X48">
         <v>48.7</v>
       </c>
     </row>
-    <row r="49">
-      <c r="A49" t="str">
-        <v>Ilya Kovalchuk</v>
+    <row r="49" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>143</v>
       </c>
       <c r="B49">
         <v>20102011</v>
       </c>
-      <c r="C49" t="str">
-        <v>NJD</v>
-      </c>
-      <c r="D49" t="str">
-        <v>R</v>
-      </c>
-      <c r="E49" t="str">
-        <v>L</v>
+      <c r="C49" t="s">
+        <v>135</v>
+      </c>
+      <c r="D49" t="s">
+        <v>30</v>
+      </c>
+      <c r="E49" t="s">
+        <v>26</v>
       </c>
       <c r="F49">
         <v>81</v>
@@ -3999,28 +4480,28 @@
       <c r="V49">
         <v>12.7</v>
       </c>
-      <c r="W49" t="str">
-        <v>22:34</v>
+      <c r="W49" t="s">
+        <v>144</v>
       </c>
       <c r="X49">
         <v>29</v>
       </c>
     </row>
-    <row r="50">
-      <c r="A50" t="str">
-        <v>Shane Doan</v>
+    <row r="50" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>145</v>
       </c>
       <c r="B50">
         <v>20102011</v>
       </c>
-      <c r="C50" t="str">
-        <v>PHX</v>
-      </c>
-      <c r="D50" t="str">
-        <v>R</v>
-      </c>
-      <c r="E50" t="str">
-        <v>R</v>
+      <c r="C50" t="s">
+        <v>146</v>
+      </c>
+      <c r="D50" t="s">
+        <v>30</v>
+      </c>
+      <c r="E50" t="s">
+        <v>30</v>
       </c>
       <c r="F50">
         <v>72</v>
@@ -4073,28 +4554,28 @@
       <c r="V50">
         <v>9.1</v>
       </c>
-      <c r="W50" t="str">
-        <v>19:17</v>
+      <c r="W50" t="s">
+        <v>74</v>
       </c>
       <c r="X50">
         <v>45.9</v>
       </c>
     </row>
-    <row r="51">
-      <c r="A51" t="str">
-        <v>Andrew Ladd</v>
+    <row r="51" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>147</v>
       </c>
       <c r="B51">
         <v>20102011</v>
       </c>
-      <c r="C51" t="str">
-        <v>ATL</v>
-      </c>
-      <c r="D51" t="str">
-        <v>L</v>
-      </c>
-      <c r="E51" t="str">
-        <v>L</v>
+      <c r="C51" t="s">
+        <v>148</v>
+      </c>
+      <c r="D51" t="s">
+        <v>26</v>
+      </c>
+      <c r="E51" t="s">
+        <v>26</v>
       </c>
       <c r="F51">
         <v>81</v>
@@ -4147,16 +4628,91 @@
       <c r="V51">
         <v>14.9</v>
       </c>
-      <c r="W51" t="str">
-        <v>20:04</v>
+      <c r="W51" t="s">
+        <v>149</v>
       </c>
       <c r="X51">
         <v>34.1</v>
       </c>
     </row>
+    <row r="52" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B52" s="1">
+        <v>20102011</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F52" s="1">
+        <v>76</v>
+      </c>
+      <c r="G52" s="1">
+        <v>11</v>
+      </c>
+      <c r="H52" s="1">
+        <v>29</v>
+      </c>
+      <c r="I52" s="1">
+        <v>40</v>
+      </c>
+      <c r="J52" s="1">
+        <v>13</v>
+      </c>
+      <c r="K52" s="1">
+        <v>68</v>
+      </c>
+      <c r="L52" s="1">
+        <v>0.53</v>
+      </c>
+      <c r="M52" s="1">
+        <v>6</v>
+      </c>
+      <c r="N52" s="1">
+        <v>25</v>
+      </c>
+      <c r="O52" s="1">
+        <v>5</v>
+      </c>
+      <c r="P52" s="1">
+        <v>15</v>
+      </c>
+      <c r="Q52" s="1">
+        <v>0</v>
+      </c>
+      <c r="R52" s="1">
+        <v>0</v>
+      </c>
+      <c r="S52" s="1">
+        <v>0</v>
+      </c>
+      <c r="T52" s="1">
+        <v>3</v>
+      </c>
+      <c r="U52" s="1">
+        <v>139</v>
+      </c>
+      <c r="V52" s="1">
+        <v>7.9</v>
+      </c>
+      <c r="W52" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="X52" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:X51"/>
+    <ignoredError sqref="A1:X51" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>